<commit_message>
Updated catalogue and tables for doc
</commit_message>
<xml_diff>
--- a/docs/CDM-manual/tables/data_catalogue_feb_2022.xlsx
+++ b/docs/CDM-manual/tables/data_catalogue_feb_2022.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\CDM\docs\CDM-manual\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\Github\CDM\docs\CDM-manual\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE21FB2-7917-49EE-A2C2-047423E88191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBEC9A70-C725-4C1C-9E74-45B09C112EF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19100" yWindow="7880" windowWidth="18500" windowHeight="9620" xr2:uid="{1CDD3442-2E6E-4676-87A8-CFE30844E482}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1CDD3442-2E6E-4676-87A8-CFE30844E482}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CDM Data Catalogue" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$R$85</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'CDM Data Catalogue'!$A$1:$R$85</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +29,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="249">
   <si>
     <t>Table</t>
   </si>
@@ -628,9 +627,6 @@
     <t>DEW Barrage</t>
   </si>
   <si>
-    <t>REVISED_FINAL_compiledBarragesData_1990-2021_Dec2021</t>
-  </si>
-  <si>
     <t>Barrage Flow</t>
   </si>
   <si>
@@ -998,6 +994,12 @@
   </si>
   <si>
     <t>Water Quality</t>
+  </si>
+  <si>
+    <t>barrage_daily_total.csv</t>
+  </si>
+  <si>
+    <t>1990 - 2022</t>
   </si>
 </sst>
 </file>
@@ -1723,25 +1725,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB9355F0-AB0C-4B99-B2F8-011B3C5C9A7E}">
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.90625" customWidth="1"/>
-    <col min="4" max="4" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="37" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1773,9 +1775,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>114</v>
@@ -1784,19 +1786,19 @@
         <v>114</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F2" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="G2" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>148</v>
-      </c>
       <c r="H2" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I2" s="6">
         <v>2021</v>
@@ -1805,9 +1807,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>114</v>
@@ -1816,19 +1818,19 @@
         <v>114</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>151</v>
-      </c>
       <c r="H3" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I3" s="6">
         <v>2021</v>
@@ -1837,9 +1839,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>114</v>
@@ -1848,19 +1850,19 @@
         <v>114</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>154</v>
-      </c>
       <c r="H4" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I4" s="6">
         <v>2018</v>
@@ -1869,9 +1871,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>114</v>
@@ -1880,37 +1882,37 @@
         <v>114</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>157</v>
-      </c>
       <c r="H5" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>63</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>64</v>
@@ -1931,18 +1933,18 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>63</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>71</v>
@@ -1961,18 +1963,18 @@
       </c>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>63</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>71</v>
@@ -1991,18 +1993,18 @@
       </c>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>63</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>77</v>
@@ -2023,18 +2025,18 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" ht="90" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>63</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>77</v>
@@ -2055,18 +2057,18 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>63</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>84</v>
@@ -2087,18 +2089,18 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>63</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>84</v>
@@ -2119,18 +2121,18 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>63</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>84</v>
@@ -2149,18 +2151,18 @@
       </c>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>63</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>84</v>
@@ -2179,18 +2181,18 @@
       </c>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" ht="90" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>63</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>77</v>
@@ -2211,18 +2213,18 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" ht="90" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>63</v>
       </c>
       <c r="C16" s="35" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>77</v>
@@ -2241,18 +2243,18 @@
       </c>
       <c r="J16" s="18"/>
     </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>111</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>120</v>
@@ -2267,56 +2269,56 @@
         <v>1</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J17" s="18" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>111</v>
       </c>
       <c r="C18" s="35" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>123</v>
       </c>
       <c r="F18" s="27" t="s">
+        <v>247</v>
+      </c>
+      <c r="G18" s="31" t="s">
         <v>124</v>
-      </c>
-      <c r="G18" s="31" t="s">
-        <v>125</v>
       </c>
       <c r="H18" s="26">
         <v>6</v>
       </c>
       <c r="I18" s="26" t="s">
-        <v>184</v>
+        <v>248</v>
       </c>
       <c r="J18" s="18" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>90</v>
       </c>
       <c r="C19" s="35" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>84</v>
@@ -2337,18 +2339,18 @@
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>90</v>
       </c>
       <c r="C20" s="35" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>84</v>
@@ -2367,18 +2369,18 @@
       </c>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>90</v>
       </c>
       <c r="C21" s="35" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>117</v>
@@ -2393,234 +2395,234 @@
         <v>1</v>
       </c>
       <c r="I21" s="26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J21" s="18" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>115</v>
       </c>
       <c r="C22" s="35" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E22" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F22" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="G22" s="28" t="s">
         <v>159</v>
-      </c>
-      <c r="G22" s="28" t="s">
-        <v>160</v>
       </c>
       <c r="H22" s="24">
         <v>2</v>
       </c>
       <c r="I22" s="24" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>115</v>
       </c>
       <c r="C23" s="35" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G23" s="28" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H23" s="5">
         <v>2</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>116</v>
       </c>
       <c r="C24" s="35" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E24" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F24" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="G24" s="12" t="s">
         <v>163</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>164</v>
       </c>
       <c r="H24" s="13">
         <v>2</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="1:10" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:10" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>113</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E25" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F25" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="F25" s="22" t="s">
+      <c r="G25" s="6" t="s">
         <v>140</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>141</v>
       </c>
       <c r="H25" s="6">
         <v>8</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>113</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D26" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F26" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="E26" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="F26" s="22" t="s">
+      <c r="G26" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="G26" s="6" t="s">
-        <v>176</v>
-      </c>
       <c r="H26" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="I26" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="I26" s="6" t="s">
-        <v>196</v>
-      </c>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>113</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G27" s="22" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H27" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="I27" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="I27" s="6" t="s">
-        <v>198</v>
-      </c>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>113</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D28" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F28" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="E28" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="F28" s="6" t="s">
+      <c r="G28" s="6" t="s">
         <v>179</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>180</v>
       </c>
       <c r="H28" s="6">
         <v>1</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>36</v>
       </c>
       <c r="C29" s="36" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>16</v>
@@ -2639,48 +2641,48 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:10" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>36</v>
       </c>
       <c r="C30" s="36" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E30" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="F30" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="G30" s="6" t="s">
         <v>144</v>
-      </c>
-      <c r="F30" s="22" t="s">
-        <v>140</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>145</v>
       </c>
       <c r="H30" s="6">
         <v>55</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J30" s="5"/>
     </row>
-    <row r="31" spans="1:10" ht="41.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:10" ht="40.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>16</v>
@@ -2701,18 +2703,18 @@
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="80" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:10" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>16</v>
@@ -2733,18 +2735,18 @@
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>16</v>
@@ -2763,18 +2765,18 @@
       </c>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>16</v>
@@ -2793,18 +2795,18 @@
       </c>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>16</v>
@@ -2825,18 +2827,18 @@
         <v>105</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>16</v>
@@ -2857,18 +2859,18 @@
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>16</v>
@@ -2889,18 +2891,18 @@
         <v>104</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>16</v>
@@ -2921,18 +2923,18 @@
         <v>105</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>16</v>
@@ -2953,18 +2955,18 @@
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>16</v>
@@ -2985,18 +2987,18 @@
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>16</v>
@@ -3017,18 +3019,18 @@
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>16</v>
@@ -3049,18 +3051,18 @@
         <v>105</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>16</v>
@@ -3081,18 +3083,18 @@
         <v>105</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>16</v>
@@ -3113,18 +3115,18 @@
         <v>105</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>16</v>
@@ -3145,18 +3147,18 @@
         <v>105</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>11</v>
@@ -3177,18 +3179,18 @@
         <v>104</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>54</v>
@@ -3209,18 +3211,18 @@
         <v>104</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D48" s="24" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>64</v>
@@ -3241,18 +3243,18 @@
         <v>107</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B49" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D49" s="24" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E49" s="14" t="s">
         <v>83</v>
@@ -3273,18 +3275,18 @@
         <v>107</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:10" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D50" s="24" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E50" s="5" t="s">
         <v>83</v>
@@ -3305,59 +3307,59 @@
         <v>107</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E51" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F51" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="F51" s="6" t="s">
+      <c r="G51" s="22" t="s">
         <v>127</v>
-      </c>
-      <c r="G51" s="22" t="s">
-        <v>128</v>
       </c>
       <c r="H51" s="6">
         <v>19</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J51" s="18" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D52" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E52" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F52" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="F52" s="6" t="s">
+      <c r="G52" s="22" t="s">
         <v>130</v>
-      </c>
-      <c r="G52" s="22" t="s">
-        <v>131</v>
       </c>
       <c r="H52" s="6">
         <v>15</v>
@@ -3369,142 +3371,142 @@
         <v>109</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D53" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E53" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="G53" s="22" t="s">
         <v>132</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G53" s="22" t="s">
-        <v>133</v>
       </c>
       <c r="H53" s="6">
         <v>19</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J53" s="18" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D54" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E54" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="F54" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="F54" s="6" t="s">
+      <c r="G54" s="29" t="s">
         <v>169</v>
-      </c>
-      <c r="G54" s="29" t="s">
-        <v>170</v>
       </c>
       <c r="H54" s="6">
         <v>1</v>
       </c>
       <c r="I54" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J54" s="5"/>
     </row>
-    <row r="55" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D55" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E55" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="F55" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="F55" s="6" t="s">
+      <c r="G55" s="6" t="s">
         <v>182</v>
-      </c>
-      <c r="G55" s="6" t="s">
-        <v>183</v>
       </c>
       <c r="H55" s="6">
         <v>20</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J55" s="20" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>112</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D56" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F56" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="G56" s="22" t="s">
         <v>137</v>
-      </c>
-      <c r="G56" s="22" t="s">
-        <v>138</v>
       </c>
       <c r="H56" s="6">
         <v>20</v>
       </c>
       <c r="I56" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J56" s="5"/>
     </row>
-    <row r="57" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>49</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D57" s="24" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E57" s="5" t="s">
         <v>50</v>
@@ -3525,18 +3527,18 @@
         <v>107</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>49</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D58" s="24" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>57</v>
@@ -3557,18 +3559,18 @@
         <v>107</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>49</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D59" s="24" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>57</v>
@@ -3589,125 +3591,125 @@
         <v>107</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B60" s="21" t="s">
         <v>49</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D60" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E60" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="F60" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="F60" s="22" t="s">
+      <c r="G60" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="G60" s="22" t="s">
-        <v>136</v>
-      </c>
       <c r="H60" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="I60" s="22" t="s">
         <v>186</v>
-      </c>
-      <c r="I60" s="22" t="s">
-        <v>187</v>
       </c>
       <c r="J60" s="18" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:10" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>49</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D61" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E61" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F61" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="G61" s="6" t="s">
         <v>142</v>
-      </c>
-      <c r="F61" s="22" t="s">
-        <v>140</v>
-      </c>
-      <c r="G61" s="6" t="s">
-        <v>143</v>
       </c>
       <c r="H61" s="6">
         <v>13</v>
       </c>
       <c r="I61" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J61" s="5"/>
     </row>
-    <row r="62" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>49</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D62" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E62" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="F62" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="F62" s="22" t="s">
+      <c r="G62" s="6" t="s">
         <v>166</v>
-      </c>
-      <c r="G62" s="6" t="s">
-        <v>167</v>
       </c>
       <c r="H62" s="6">
         <v>2</v>
       </c>
       <c r="I62" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J62" s="5"/>
     </row>
-    <row r="63" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>49</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D63" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E63" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F63" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="F63" s="6" t="s">
+      <c r="G63" s="22" t="s">
         <v>172</v>
-      </c>
-      <c r="G63" s="22" t="s">
-        <v>173</v>
       </c>
       <c r="H63" s="6">
         <v>3</v>
       </c>
       <c r="I63" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J63" s="5"/>
     </row>

</xml_diff>